<commit_message>
Updating average results for graphs with 10 to 90 vertices.
</commit_message>
<xml_diff>
--- a/result/Speedup results - V2.xlsx
+++ b/result/Speedup results - V2.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="72">
   <si>
     <t>n</t>
   </si>
@@ -150,10 +150,19 @@
     <t>Media lower bound</t>
   </si>
   <si>
+    <t>10-90 Vertices</t>
+  </si>
+  <si>
     <t>H1</t>
   </si>
   <si>
     <t>H2</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>STD</t>
   </si>
   <si>
     <t>Barabasi-Albert</t>
@@ -347,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -437,6 +446,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="4" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -969,11 +981,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="796782486"/>
-        <c:axId val="402059930"/>
+        <c:axId val="117442018"/>
+        <c:axId val="318315813"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="796782486"/>
+        <c:axId val="117442018"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1025,10 +1037,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="402059930"/>
+        <c:crossAx val="318315813"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="402059930"/>
+        <c:axId val="318315813"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -1104,7 +1116,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="796782486"/>
+        <c:crossAx val="117442018"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1332,11 +1344,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="561375813"/>
-        <c:axId val="1336679180"/>
+        <c:axId val="1800783744"/>
+        <c:axId val="441172202"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="561375813"/>
+        <c:axId val="1800783744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1388,10 +1400,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1336679180"/>
+        <c:crossAx val="441172202"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1336679180"/>
+        <c:axId val="441172202"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1455,7 +1467,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="561375813"/>
+        <c:crossAx val="1800783744"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1683,11 +1695,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="656620691"/>
-        <c:axId val="1972110152"/>
+        <c:axId val="1924463172"/>
+        <c:axId val="1331107802"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="656620691"/>
+        <c:axId val="1924463172"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1739,10 +1751,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1972110152"/>
+        <c:crossAx val="1331107802"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1972110152"/>
+        <c:axId val="1331107802"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1817,7 +1829,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="656620691"/>
+        <c:crossAx val="1924463172"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2045,11 +2057,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1101045425"/>
-        <c:axId val="1865206876"/>
+        <c:axId val="538479528"/>
+        <c:axId val="1386801568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1101045425"/>
+        <c:axId val="538479528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2101,10 +2113,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1865206876"/>
+        <c:crossAx val="1386801568"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1865206876"/>
+        <c:axId val="1386801568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2179,7 +2191,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1101045425"/>
+        <c:crossAx val="538479528"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -33250,51 +33262,82 @@
       <c r="D727" s="17" t="s">
         <v>44</v>
       </c>
+      <c r="H727" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="I727" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="J727" s="17" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="728">
       <c r="A728" s="17">
         <v>100.0</v>
       </c>
-      <c r="B728" s="32">
+      <c r="B728" s="33">
         <f>AVERAGE(C92:C101,C282:C291,C472:C481,C622:C631)</f>
         <v>1905.4</v>
       </c>
       <c r="D728" s="17">
         <v>100.0</v>
       </c>
-      <c r="E728" s="32">
+      <c r="E728" s="33">
         <f>AVERAGE(D92:D101,D282:D291,D472:D481,D622:D631)</f>
         <v>2.25</v>
+      </c>
+      <c r="H728" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="I728" s="33">
+        <f t="shared" ref="I728:J728" si="1">AVERAGE(I2:I91,I192:I281,I382:I471,I572:I621)</f>
+        <v>2.359375</v>
+      </c>
+      <c r="J728" s="33">
+        <f t="shared" si="1"/>
+        <v>1.9375</v>
       </c>
     </row>
     <row r="729">
       <c r="A729" s="17">
         <v>200.0</v>
       </c>
-      <c r="B729" s="32">
+      <c r="B729" s="33">
         <f>AVERAGE(C102:C112,C293:C301,C482:C491,C632:C641)</f>
         <v>7928.875</v>
       </c>
       <c r="D729" s="17">
         <v>200.0</v>
       </c>
-      <c r="E729" s="32">
+      <c r="E729" s="33">
         <f>AVERAGE(D102:D111,D292:D301,D482:D491,D632:D641)</f>
         <v>2.25</v>
+      </c>
+      <c r="H729" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="I729" s="25">
+        <f t="shared" ref="I729:J729" si="2">_xlfn.STDEV.P(I2:I91,I192:I281,I382:I471,I572:I621)</f>
+        <v>1.495484741</v>
+      </c>
+      <c r="J729" s="25">
+        <f t="shared" si="2"/>
+        <v>1.248436522</v>
       </c>
     </row>
     <row r="730">
       <c r="A730" s="17">
         <v>300.0</v>
       </c>
-      <c r="B730" s="32">
+      <c r="B730" s="33">
         <f>AVERAGE(C112:C121,C302:C311,C492:C501,C642:C651)</f>
         <v>17176.2</v>
       </c>
       <c r="D730" s="17">
         <v>300.0</v>
       </c>
-      <c r="E730" s="32">
+      <c r="E730" s="33">
         <f>AVERAGE(D112:D121,D302:D311,D492:D501,D642:D651)</f>
         <v>2.25</v>
       </c>
@@ -33303,14 +33346,14 @@
       <c r="A731" s="17">
         <v>400.0</v>
       </c>
-      <c r="B731" s="32">
+      <c r="B731" s="33">
         <f>AVERAGE(C122:C130,C312:C321,C502:C511,C652:C661)</f>
         <v>30369.15385</v>
       </c>
       <c r="D731" s="17">
         <v>400.0</v>
       </c>
-      <c r="E731" s="32">
+      <c r="E731" s="33">
         <f>AVERAGE(D122:D131,D312:D321,D502:D511,D652:D661)</f>
         <v>2.25</v>
       </c>
@@ -33319,14 +33362,14 @@
       <c r="A732" s="17">
         <v>500.0</v>
       </c>
-      <c r="B732" s="32">
+      <c r="B732" s="33">
         <f>AVERAGE(C132:C141,C322:C331,C512:C521,C662:C671)</f>
         <v>47776.375</v>
       </c>
       <c r="D732" s="17">
         <v>500.0</v>
       </c>
-      <c r="E732" s="32">
+      <c r="E732" s="33">
         <f>AVERAGE(D132:D141,D322:D331,D512:D521,D662:D671)</f>
         <v>2.25</v>
       </c>
@@ -33335,7 +33378,7 @@
       <c r="A733" s="17">
         <v>600.0</v>
       </c>
-      <c r="B733" s="32">
+      <c r="B733" s="33">
         <f>AVERAGE(C142:C151,C332:C341,C522:C531,C672:C681)</f>
         <v>68815.75</v>
       </c>
@@ -33347,7 +33390,7 @@
       <c r="A734" s="17">
         <v>700.0</v>
       </c>
-      <c r="B734" s="32">
+      <c r="B734" s="33">
         <f>AVERAGE(C152:C161,C342:C351,C532:C541,C682:C691)</f>
         <v>93691.15</v>
       </c>
@@ -33359,7 +33402,7 @@
       <c r="A735" s="17">
         <v>800.0</v>
       </c>
-      <c r="B735" s="32">
+      <c r="B735" s="33">
         <f>AVERAGE(C162:C171,C352:C361,C542:C550,C692:C701)</f>
         <v>122159.4872</v>
       </c>
@@ -33371,7 +33414,7 @@
       <c r="A736" s="17">
         <v>900.0</v>
       </c>
-      <c r="B736" s="32">
+      <c r="B736" s="33">
         <f>AVERAGE(C172:C181,C362:C371,C552:C561,C702:C711)</f>
         <v>154851.175</v>
       </c>
@@ -33383,7 +33426,7 @@
       <c r="A737" s="17">
         <v>1000.0</v>
       </c>
-      <c r="B737" s="32">
+      <c r="B737" s="33">
         <f>AVERAGE(C182:C191,C372:C381,C562:C571,C712:C721)</f>
         <v>191191.35</v>
       </c>
@@ -33393,56 +33436,56 @@
     </row>
     <row r="742">
       <c r="C742" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M742" s="17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="743">
-      <c r="A743" s="33"/>
-      <c r="B743" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="C743" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="D743" s="34" t="s">
-        <v>49</v>
+      <c r="A743" s="34"/>
+      <c r="B743" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="C743" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="D743" s="35" t="s">
+        <v>52</v>
       </c>
       <c r="E743" s="27" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G743" s="27"/>
       <c r="I743" s="27"/>
-      <c r="K743" s="33"/>
-      <c r="L743" s="34" t="s">
-        <v>47</v>
+      <c r="K743" s="34"/>
+      <c r="L743" s="35" t="s">
+        <v>50</v>
       </c>
       <c r="M743" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="N743" s="34" t="s">
-        <v>49</v>
+        <v>51</v>
+      </c>
+      <c r="N743" s="35" t="s">
+        <v>52</v>
       </c>
       <c r="O743" s="27" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="P743" s="27"/>
       <c r="Q743" s="27"/>
       <c r="R743" s="27"/>
-      <c r="S743" s="33"/>
-      <c r="T743" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="U743" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="V743" s="34" t="s">
-        <v>49</v>
+      <c r="S743" s="34"/>
+      <c r="T743" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="U743" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="V743" s="35" t="s">
+        <v>52</v>
       </c>
       <c r="W743" s="27" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="744">
@@ -33461,8 +33504,8 @@
       <c r="E744" s="27">
         <v>0.0359623</v>
       </c>
-      <c r="G744" s="35"/>
-      <c r="I744" s="35"/>
+      <c r="G744" s="36"/>
+      <c r="I744" s="36"/>
       <c r="J744" s="10"/>
       <c r="K744" s="30">
         <v>100.0</v>
@@ -33473,32 +33516,32 @@
       <c r="M744" s="30">
         <v>0.08335</v>
       </c>
-      <c r="N744" s="36">
+      <c r="N744" s="37">
         <v>6.65499999999999E-5</v>
       </c>
-      <c r="O744" s="36">
+      <c r="O744" s="37">
         <v>6.72E-5</v>
       </c>
       <c r="P744" s="27"/>
-      <c r="Q744" s="35"/>
+      <c r="Q744" s="36"/>
       <c r="R744" s="27"/>
       <c r="S744" s="30">
         <v>100.0</v>
       </c>
       <c r="T744" s="27">
-        <f t="shared" ref="T744:W744" si="1">B744/L744</f>
+        <f t="shared" ref="T744:W744" si="3">B744/L744</f>
         <v>0.2578101033</v>
       </c>
       <c r="U744" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.5381046191</v>
       </c>
-      <c r="V744" s="35">
-        <f t="shared" si="1"/>
+      <c r="V744" s="36">
+        <f t="shared" si="3"/>
         <v>469.664012</v>
       </c>
-      <c r="W744" s="35">
-        <f t="shared" si="1"/>
+      <c r="W744" s="36">
+        <f t="shared" si="3"/>
         <v>535.1532738</v>
       </c>
     </row>
@@ -33542,19 +33585,19 @@
         <v>200.0</v>
       </c>
       <c r="T745" s="27">
-        <f t="shared" ref="T745:W745" si="2">B745/L745</f>
+        <f t="shared" ref="T745:W745" si="4">B745/L745</f>
         <v>652.5126181</v>
       </c>
       <c r="U745" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1097.621014</v>
       </c>
       <c r="V745" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1238.208101</v>
       </c>
       <c r="W745" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1360.169735</v>
       </c>
     </row>
@@ -33598,19 +33641,19 @@
         <v>300.0</v>
       </c>
       <c r="T746" s="27">
-        <f t="shared" ref="T746:W746" si="3">B746/L746</f>
+        <f t="shared" ref="T746:W746" si="5">B746/L746</f>
         <v>1907.89496</v>
       </c>
       <c r="U746" s="27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1575.694714</v>
       </c>
       <c r="V746" s="27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2019.579496</v>
       </c>
       <c r="W746" s="27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2073.720321</v>
       </c>
     </row>
@@ -33654,19 +33697,19 @@
         <v>400.0</v>
       </c>
       <c r="T747" s="27">
-        <f t="shared" ref="T747:W747" si="4">B747/L747</f>
+        <f t="shared" ref="T747:W747" si="6">B747/L747</f>
         <v>2407.264221</v>
       </c>
       <c r="U747" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2283.825514</v>
       </c>
       <c r="V747" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2869.032142</v>
       </c>
       <c r="W747" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2929.565167</v>
       </c>
     </row>
@@ -33710,19 +33753,19 @@
         <v>500.0</v>
       </c>
       <c r="T748" s="27">
-        <f t="shared" ref="T748:W748" si="5">B748/L748</f>
+        <f t="shared" ref="T748:W748" si="7">B748/L748</f>
         <v>3371.42876</v>
       </c>
       <c r="U748" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2630.801884</v>
       </c>
       <c r="V748" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5520.409725</v>
       </c>
       <c r="W748" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3843.40301</v>
       </c>
     </row>
@@ -33766,19 +33809,19 @@
         <v>600.0</v>
       </c>
       <c r="T749" s="27">
-        <f t="shared" ref="T749:W749" si="6">B749/L749</f>
+        <f t="shared" ref="T749:W749" si="8">B749/L749</f>
         <v>4800.114429</v>
       </c>
       <c r="U749" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3098.816089</v>
       </c>
       <c r="V749" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>6536.484445</v>
       </c>
       <c r="W749" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>6584.863645</v>
       </c>
     </row>
@@ -33822,19 +33865,19 @@
         <v>700.0</v>
       </c>
       <c r="T750" s="27">
-        <f t="shared" ref="T750:W750" si="7">B750/L750</f>
+        <f t="shared" ref="T750:W750" si="9">B750/L750</f>
         <v>5639.066427</v>
       </c>
       <c r="U750" s="27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3860.219147</v>
       </c>
       <c r="V750" s="27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>7470.315093</v>
       </c>
       <c r="W750" s="27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>7320.785813</v>
       </c>
     </row>
@@ -33878,19 +33921,19 @@
         <v>800.0</v>
       </c>
       <c r="T751" s="27">
-        <f t="shared" ref="T751:W751" si="8">B751/L751</f>
+        <f t="shared" ref="T751:W751" si="10">B751/L751</f>
         <v>6205.754177</v>
       </c>
       <c r="U751" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>4360.029661</v>
       </c>
       <c r="V751" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>8270.008688</v>
       </c>
       <c r="W751" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>8605.346728</v>
       </c>
     </row>
@@ -33934,19 +33977,19 @@
         <v>900.0</v>
       </c>
       <c r="T752" s="27">
-        <f t="shared" ref="T752:W752" si="9">B752/L752</f>
+        <f t="shared" ref="T752:W752" si="11">B752/L752</f>
         <v>7565.600833</v>
       </c>
       <c r="U752" s="27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>4838.889892</v>
       </c>
       <c r="V752" s="27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>10452.08219</v>
       </c>
       <c r="W752" s="27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>9644.807799</v>
       </c>
     </row>
@@ -33990,19 +34033,19 @@
         <v>1000.0</v>
       </c>
       <c r="T753" s="27">
-        <f t="shared" ref="T753:W753" si="10">B753/L753</f>
+        <f t="shared" ref="T753:W753" si="12">B753/L753</f>
         <v>8177.396999</v>
       </c>
       <c r="U753" s="27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>5191.500369</v>
       </c>
       <c r="V753" s="27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>11202.94929</v>
       </c>
       <c r="W753" s="27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>11378.17989</v>
       </c>
     </row>
@@ -34027,106 +34070,106 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="37" t="s">
+      <c r="A1" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="37" t="s">
-        <v>54</v>
-      </c>
-      <c r="G1" s="37" t="s">
-        <v>55</v>
+      <c r="E1" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="38" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="37" t="s">
+      <c r="B2" s="38" t="s">
         <v>59</v>
       </c>
+      <c r="C2" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="38" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="D3" s="40"/>
-      <c r="E3" s="39">
+      <c r="D3" s="41"/>
+      <c r="E3" s="40">
         <v>50.0</v>
       </c>
-      <c r="F3" s="40"/>
-      <c r="G3" s="39" t="s">
+      <c r="F3" s="41"/>
+      <c r="G3" s="40" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="41"/>
+      <c r="E4" s="40">
+        <v>30.0</v>
+      </c>
+      <c r="F4" s="40" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="D4" s="40"/>
-      <c r="E4" s="39">
+      <c r="G4" s="40" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="40">
         <v>30.0</v>
       </c>
-      <c r="F4" s="39" t="s">
-        <v>58</v>
-      </c>
-      <c r="G4" s="39" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="39" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="D5" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" s="39">
-        <v>30.0</v>
-      </c>
-      <c r="F5" s="40"/>
-      <c r="G5" s="39" t="s">
-        <v>68</v>
+      <c r="F5" s="41"/>
+      <c r="G5" s="40" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>